<commit_message>
project func: Update gem5&M1&host compare Excel.
Update the gem5 ckp vs M1 ckp error comparison to both using valid ckp, with the relevant data for gem5 using column D in the sheet Summary.
Adjust the alignment style of the cells in columns E, H, and I of sheet host-IPC&CPI to be centered
</commit_message>
<xml_diff>
--- a/data/meta/gem5_statistics_result_template.xlsx
+++ b/data/meta/gem5_statistics_result_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15820"/>
+    <workbookView windowWidth="30080" windowHeight="14780"/>
   </bookViews>
   <sheets>
     <sheet name="host-IPC&amp;CPI" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t>gem5 ckp ipc</t>
   </si>
   <si>
-    <t>gem5 ckp与完整跑</t>
+    <t>gem5 ckp与完整跑误差</t>
   </si>
   <si>
     <t>ckp与M1 ckp误差</t>
@@ -58,10 +58,10 @@
     <t>gem5运行时间</t>
   </si>
   <si>
-    <t>GEM5 CPI</t>
-  </si>
-  <si>
-    <t>M1 CPI</t>
+    <t>gem5 ckp CPI</t>
+  </si>
+  <si>
+    <t>M1 ckp CPI</t>
   </si>
   <si>
     <t>有效ckp占比</t>
@@ -163,9 +163,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -212,7 +212,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -226,6 +226,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -234,23 +242,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -260,35 +253,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,7 +268,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,15 +284,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -335,7 +306,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,169 +374,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,31 +756,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -815,21 +806,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -840,147 +816,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1439,8 +1439,8 @@
   <sheetPr/>
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18269230769231" defaultRowHeight="16.8"/>
@@ -1453,13 +1453,13 @@
     <col min="6" max="6" width="19.2692307692308" customWidth="1"/>
     <col min="7" max="7" width="15.3653846153846" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.0865384615385" customWidth="1"/>
-    <col min="9" max="9" width="19.7307692307692" customWidth="1"/>
+    <col min="9" max="9" width="24.3076923076923" customWidth="1"/>
     <col min="10" max="10" width="16.5384615384615" style="2" customWidth="1"/>
     <col min="11" max="11" width="13.6346153846154" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.3653846153846" style="2" customWidth="1"/>
     <col min="13" max="13" width="16.2692307692308" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.8461538461538" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.18269230769231" style="2"/>
+    <col min="14" max="14" width="17.2307692307692" style="2" customWidth="1"/>
+    <col min="15" max="15" width="13.6923076923077" style="2" customWidth="1"/>
     <col min="16" max="16" width="20.0865384615385" style="2" customWidth="1"/>
     <col min="17" max="16384" width="9.18269230769231" style="2"/>
   </cols>
@@ -2823,7 +2823,7 @@
         <v>56.036</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" ht="17.55" spans="1:16">
       <c r="A25" s="8" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
project func: Update Excel "GEOMEAN" and "AVERAGE" formula
Exclude 999
Fixup P<M1 ckp CPI>,G<m1 ckp ipc> columns formula
</commit_message>
<xml_diff>
--- a/data/meta/gem5_statistics_result_template.xlsx
+++ b/data/meta/gem5_statistics_result_template.xlsx
@@ -213,10 +213,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -249,14 +249,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,7 +295,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,23 +332,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -316,37 +348,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -355,7 +356,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,25 +378,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -431,25 +431,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,49 +443,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,13 +467,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,7 +521,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,49 +575,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,30 +846,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -902,6 +878,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -947,157 +938,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1129,9 +1129,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1253,9 +1250,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="46" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1604,10 +1598,10 @@
   <sheetPr/>
   <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18269230769231" defaultRowHeight="16.8"/>
@@ -1687,7 +1681,7 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1702,7 +1696,7 @@
       <c r="D2" s="5">
         <v>1.705499</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <f>IFERROR((D2-B2)/B2,0)</f>
         <v>0.39795</v>
       </c>
@@ -1711,30 +1705,30 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="e">
-        <f>1/O2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H2" s="24" t="e">
+        <f>1/P2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H2" s="23" t="e">
         <f>1/N2</f>
         <v>#REF!</v>
       </c>
-      <c r="I2" s="24" t="e">
+      <c r="I2" s="23" t="e">
         <f>(H2-D2)/D2</f>
         <v>#REF!</v>
       </c>
-      <c r="J2" s="36">
+      <c r="J2" s="35">
         <f t="shared" ref="J2:J25" si="0">IFERROR((H2-G2)/G2,1)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="36">
+      <c r="K2" s="35">
         <f t="shared" ref="K2:K25" si="1">IFERROR((H2-B2)/B2,1)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="36">
+      <c r="L2" s="35">
         <f t="shared" ref="L2:L25" si="2">IFERROR((H2-C2)/C2,1)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="50">
+      <c r="M2" s="49">
         <v>0.345219907407407</v>
       </c>
       <c r="N2" s="2" t="e">
@@ -1745,8 +1739,9 @@
         <f>[1]summaryCPI!D2</f>
         <v>#REF!</v>
       </c>
-      <c r="P2" s="2">
-        <v>0.456226</v>
+      <c r="P2" s="2" t="e">
+        <f>[1]summaryCPI!C2</f>
+        <v>#REF!</v>
       </c>
       <c r="Q2" s="2">
         <f t="shared" ref="Q2:Q9" si="3">1/D2</f>
@@ -1773,7 +1768,7 @@
       <c r="D3" s="5">
         <v>0.995271</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <f t="shared" ref="E3:E25" si="5">IFERROR((D3-B3)/B3,0)</f>
         <v>0.00532424242424245</v>
       </c>
@@ -1782,30 +1777,30 @@
         <v>-0.0727173629486081</v>
       </c>
       <c r="G3" s="5" t="e">
-        <f t="shared" ref="G3:G25" si="7">1/O3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H3" s="24" t="e">
+        <f t="shared" ref="G3:G25" si="7">1/P3</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H3" s="23" t="e">
         <f t="shared" ref="H3:H25" si="8">1/N3</f>
         <v>#REF!</v>
       </c>
-      <c r="I3" s="24" t="e">
+      <c r="I3" s="23" t="e">
         <f t="shared" ref="I3:I25" si="9">(H3-D3)/D3</f>
         <v>#REF!</v>
       </c>
-      <c r="J3" s="36">
+      <c r="J3" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K3" s="36">
+      <c r="K3" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L3" s="36">
+      <c r="L3" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M3" s="51">
+      <c r="M3" s="50">
         <v>0.15625</v>
       </c>
       <c r="N3" s="2" t="e">
@@ -1816,8 +1811,9 @@
         <f>[1]summaryCPI!D3</f>
         <v>#REF!</v>
       </c>
-      <c r="P3" s="2">
-        <v>0.83601</v>
+      <c r="P3" s="2" t="e">
+        <f>[1]summaryCPI!C3</f>
+        <v>#REF!</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" si="3"/>
@@ -1842,7 +1838,7 @@
       <c r="D4" s="5">
         <v>0.847509</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <f t="shared" si="5"/>
         <v>0.345252380952381</v>
       </c>
@@ -1854,27 +1850,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H4" s="24" t="e">
+      <c r="H4" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I4" s="24" t="e">
+      <c r="I4" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K4" s="36">
+      <c r="K4" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L4" s="36">
+      <c r="L4" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M4" s="52">
+      <c r="M4" s="51">
         <v>4.57329861111111</v>
       </c>
       <c r="N4" s="2" t="e">
@@ -1885,8 +1881,9 @@
         <f>[1]summaryCPI!D4</f>
         <v>#REF!</v>
       </c>
-      <c r="P4" s="2">
-        <v>0.86706</v>
+      <c r="P4" s="2" t="e">
+        <f>[1]summaryCPI!C4</f>
+        <v>#REF!</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="3"/>
@@ -1911,7 +1908,7 @@
       <c r="D5" s="5">
         <v>0.836</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="22">
         <f t="shared" ref="E5:E12" si="10">IFERROR((D5-B5)/B5,0)</f>
         <v>-0.0593530239099859</v>
       </c>
@@ -1923,27 +1920,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H5" s="24" t="e">
+      <c r="H5" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I5" s="24" t="e">
+      <c r="I5" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J5" s="36">
+      <c r="J5" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L5" s="36">
+      <c r="L5" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M5" s="52">
+      <c r="M5" s="51">
         <v>2.32777777777778</v>
       </c>
       <c r="N5" s="2" t="e">
@@ -1954,8 +1951,9 @@
         <f>[1]summaryCPI!D5</f>
         <v>#REF!</v>
       </c>
-      <c r="P5" s="2">
-        <v>0.515899</v>
+      <c r="P5" s="2" t="e">
+        <f>[1]summaryCPI!C5</f>
+        <v>#REF!</v>
       </c>
       <c r="Q5" s="2">
         <f t="shared" si="3"/>
@@ -1982,7 +1980,7 @@
       <c r="D6" s="5">
         <v>0.831469</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="22">
         <f t="shared" si="10"/>
         <v>-0.208124761904762</v>
       </c>
@@ -1994,27 +1992,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="24" t="e">
+      <c r="H6" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I6" s="24" t="e">
+      <c r="I6" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J6" s="36">
+      <c r="J6" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K6" s="36">
+      <c r="K6" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L6" s="36">
+      <c r="L6" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M6" s="50">
+      <c r="M6" s="49">
         <v>0.058287037037037</v>
       </c>
       <c r="N6" s="2" t="e">
@@ -2025,8 +2023,9 @@
         <f>[1]summaryCPI!D6</f>
         <v>#REF!</v>
       </c>
-      <c r="P6" s="2">
-        <v>0.899467</v>
+      <c r="P6" s="2" t="e">
+        <f>[1]summaryCPI!C6</f>
+        <v>#REF!</v>
       </c>
       <c r="Q6" s="2">
         <f t="shared" si="3"/>
@@ -2051,7 +2050,7 @@
       <c r="D7" s="5">
         <v>1.797233</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <f t="shared" si="10"/>
         <v>0.214346621621622</v>
       </c>
@@ -2063,27 +2062,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H7" s="24" t="e">
+      <c r="H7" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I7" s="24" t="e">
+      <c r="I7" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L7" s="36">
+      <c r="L7" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M7" s="50">
+      <c r="M7" s="49">
         <v>0.221099537037037</v>
       </c>
       <c r="N7" s="2" t="e">
@@ -2094,8 +2093,9 @@
         <f>[1]summaryCPI!D7</f>
         <v>#REF!</v>
       </c>
-      <c r="P7" s="2">
-        <v>0.680909</v>
+      <c r="P7" s="2" t="e">
+        <f>[1]summaryCPI!C7</f>
+        <v>#REF!</v>
       </c>
       <c r="Q7" s="2">
         <f t="shared" si="3"/>
@@ -2120,7 +2120,7 @@
       <c r="D8" s="5">
         <v>1.152525</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <f t="shared" si="10"/>
         <v>-0.126875</v>
       </c>
@@ -2132,27 +2132,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H8" s="24" t="e">
+      <c r="H8" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I8" s="24" t="e">
+      <c r="I8" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J8" s="36">
+      <c r="J8" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L8" s="36">
+      <c r="L8" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M8" s="52">
+      <c r="M8" s="51">
         <v>5.38105324074074</v>
       </c>
       <c r="N8" s="2" t="e">
@@ -2163,8 +2163,9 @@
         <f>[1]summaryCPI!D8</f>
         <v>#REF!</v>
       </c>
-      <c r="P8" s="2">
-        <v>0.597612</v>
+      <c r="P8" s="2" t="e">
+        <f>[1]summaryCPI!C8</f>
+        <v>#REF!</v>
       </c>
       <c r="Q8" s="2">
         <f t="shared" si="3"/>
@@ -2189,7 +2190,7 @@
       <c r="D9" s="5">
         <v>0.932275</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="22">
         <f t="shared" si="10"/>
         <v>-0.22952479338843</v>
       </c>
@@ -2201,23 +2202,23 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H9" s="24" t="e">
+      <c r="H9" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I9" s="24" t="e">
+      <c r="I9" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J9" s="36">
+      <c r="J9" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K9" s="36">
+      <c r="K9" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L9" s="36">
+      <c r="L9" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2230,8 +2231,9 @@
         <f>[1]summaryCPI!D9</f>
         <v>#REF!</v>
       </c>
-      <c r="P9" s="2">
-        <v>0.31359</v>
+      <c r="P9" s="2" t="e">
+        <f>[1]summaryCPI!C9</f>
+        <v>#REF!</v>
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="3"/>
@@ -2254,7 +2256,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
@@ -2266,27 +2268,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H10" s="24" t="e">
+      <c r="H10" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I10" s="24" t="e">
+      <c r="I10" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J10" s="36">
+      <c r="J10" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K10" s="36">
+      <c r="K10" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L10" s="36">
+      <c r="L10" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M10" s="52">
+      <c r="M10" s="51">
         <v>7.96752314814815</v>
       </c>
       <c r="N10" s="2" t="e">
@@ -2297,8 +2299,9 @@
         <f>[1]summaryCPI!D10</f>
         <v>#REF!</v>
       </c>
-      <c r="P10" s="2">
-        <v>0.254914</v>
+      <c r="P10" s="2" t="e">
+        <f>[1]summaryCPI!C10</f>
+        <v>#REF!</v>
       </c>
       <c r="Q10" s="2">
         <v>0</v>
@@ -2324,7 +2327,7 @@
       <c r="D11" s="5">
         <v>1.415113</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <f t="shared" si="10"/>
         <v>0.0600097378277153</v>
       </c>
@@ -2336,27 +2339,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H11" s="24" t="e">
+      <c r="H11" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I11" s="24" t="e">
+      <c r="I11" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J11" s="36">
+      <c r="J11" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K11" s="36">
+      <c r="K11" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M11" s="50">
+      <c r="M11" s="49">
         <v>0.0677083333333333</v>
       </c>
       <c r="N11" s="2" t="e">
@@ -2367,8 +2370,9 @@
         <f>[1]summaryCPI!D11</f>
         <v>#REF!</v>
       </c>
-      <c r="P11" s="2">
-        <v>0.842071</v>
+      <c r="P11" s="2" t="e">
+        <f>[1]summaryCPI!C11</f>
+        <v>#REF!</v>
       </c>
       <c r="Q11" s="2">
         <f t="shared" ref="Q11:Q19" si="12">1/D11</f>
@@ -2393,7 +2397,7 @@
       <c r="D12" s="5">
         <v>0.505629</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <f t="shared" si="10"/>
         <v>-0.307357534246575</v>
       </c>
@@ -2405,27 +2409,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H12" s="24" t="e">
+      <c r="H12" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I12" s="24" t="e">
+      <c r="I12" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J12" s="36">
+      <c r="J12" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K12" s="36">
+      <c r="K12" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L12" s="36">
+      <c r="L12" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M12" s="52">
+      <c r="M12" s="51">
         <v>2.1987962962963</v>
       </c>
       <c r="N12" s="2" t="e">
@@ -2436,8 +2440,9 @@
         <f>[1]summaryCPI!D12</f>
         <v>#REF!</v>
       </c>
-      <c r="P12" s="2">
-        <v>2.37418</v>
+      <c r="P12" s="2" t="e">
+        <f>[1]summaryCPI!C12</f>
+        <v>#REF!</v>
       </c>
       <c r="Q12" s="2">
         <f t="shared" si="12"/>
@@ -2462,7 +2467,7 @@
       <c r="D13" s="5">
         <v>0.727417</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <f t="shared" si="5"/>
         <v>0.499828865979382</v>
       </c>
@@ -2474,27 +2479,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H13" s="24" t="e">
+      <c r="H13" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I13" s="24" t="e">
+      <c r="I13" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J13" s="36">
+      <c r="J13" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K13" s="36">
+      <c r="K13" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L13" s="36">
+      <c r="L13" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M13" s="52">
+      <c r="M13" s="51">
         <v>3.10461805555556</v>
       </c>
       <c r="N13" s="2" t="e">
@@ -2505,8 +2510,9 @@
         <f>[1]summaryCPI!D13</f>
         <v>#REF!</v>
       </c>
-      <c r="P13" s="2">
-        <v>0.859784</v>
+      <c r="P13" s="2" t="e">
+        <f>[1]summaryCPI!C13</f>
+        <v>#REF!</v>
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="12"/>
@@ -2531,7 +2537,7 @@
       <c r="D14" s="5">
         <v>1.390743</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <f t="shared" si="5"/>
         <v>-0.244161413043478</v>
       </c>
@@ -2543,27 +2549,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H14" s="24" t="e">
+      <c r="H14" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I14" s="24" t="e">
+      <c r="I14" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J14" s="36">
+      <c r="J14" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K14" s="36">
+      <c r="K14" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L14" s="36">
+      <c r="L14" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M14" s="52">
+      <c r="M14" s="51">
         <v>7.72336805555556</v>
       </c>
       <c r="N14" s="2" t="e">
@@ -2574,8 +2580,9 @@
         <f>[1]summaryCPI!D14</f>
         <v>#REF!</v>
       </c>
-      <c r="P14" s="2">
-        <v>0.30065</v>
+      <c r="P14" s="2" t="e">
+        <f>[1]summaryCPI!C14</f>
+        <v>#REF!</v>
       </c>
       <c r="Q14" s="2">
         <f t="shared" si="12"/>
@@ -2600,7 +2607,7 @@
       <c r="D15" s="5">
         <v>1.174566</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="22">
         <f t="shared" si="5"/>
         <v>-0.0733207100591715</v>
       </c>
@@ -2612,27 +2619,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H15" s="24" t="e">
+      <c r="H15" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I15" s="24" t="e">
+      <c r="I15" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J15" s="36">
+      <c r="J15" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K15" s="36">
+      <c r="K15" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L15" s="36">
+      <c r="L15" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M15" s="52">
+      <c r="M15" s="51">
         <v>3.00680555555556</v>
       </c>
       <c r="N15" s="2" t="e">
@@ -2643,8 +2650,9 @@
         <f>[1]summaryCPI!D15</f>
         <v>#REF!</v>
       </c>
-      <c r="P15" s="2">
-        <v>0.737944</v>
+      <c r="P15" s="2" t="e">
+        <f>[1]summaryCPI!C15</f>
+        <v>#REF!</v>
       </c>
       <c r="Q15" s="2">
         <f t="shared" si="12"/>
@@ -2669,7 +2677,7 @@
       <c r="D16" s="5">
         <v>1.030133</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <f t="shared" si="5"/>
         <v>-0.134342016806723</v>
       </c>
@@ -2681,27 +2689,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H16" s="24" t="e">
+      <c r="H16" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I16" s="24" t="e">
+      <c r="I16" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J16" s="36">
+      <c r="J16" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K16" s="36">
+      <c r="K16" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L16" s="36">
+      <c r="L16" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M16" s="50">
+      <c r="M16" s="49">
         <v>0.409791666666667</v>
       </c>
       <c r="N16" s="2" t="e">
@@ -2712,8 +2720,9 @@
         <f>[1]summaryCPI!D16</f>
         <v>#REF!</v>
       </c>
-      <c r="P16" s="2">
-        <v>0.733757</v>
+      <c r="P16" s="2" t="e">
+        <f>[1]summaryCPI!C16</f>
+        <v>#REF!</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="12"/>
@@ -2738,7 +2747,7 @@
       <c r="D17" s="5">
         <v>0.477309</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <f t="shared" si="5"/>
         <v>-0.569991891891892</v>
       </c>
@@ -2750,27 +2759,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H17" s="24" t="e">
+      <c r="H17" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I17" s="24" t="e">
+      <c r="I17" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J17" s="36">
+      <c r="J17" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K17" s="36">
+      <c r="K17" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L17" s="36">
+      <c r="L17" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M17" s="50">
+      <c r="M17" s="49">
         <v>0.837685185185185</v>
       </c>
       <c r="N17" s="2" t="e">
@@ -2781,8 +2790,9 @@
         <f>[1]summaryCPI!D17</f>
         <v>#REF!</v>
       </c>
-      <c r="P17" s="2">
-        <v>1.61859</v>
+      <c r="P17" s="2" t="e">
+        <f>[1]summaryCPI!C17</f>
+        <v>#REF!</v>
       </c>
       <c r="Q17" s="2">
         <f t="shared" si="12"/>
@@ -2807,7 +2817,7 @@
       <c r="D18" s="5">
         <v>0.650208</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <f t="shared" si="5"/>
         <v>-0.343224242424242</v>
       </c>
@@ -2819,27 +2829,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H18" s="24" t="e">
+      <c r="H18" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I18" s="24" t="e">
+      <c r="I18" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J18" s="36">
+      <c r="J18" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K18" s="36">
+      <c r="K18" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L18" s="36">
+      <c r="L18" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M18" s="52">
+      <c r="M18" s="51">
         <v>6.69226851851852</v>
       </c>
       <c r="N18" s="2" t="e">
@@ -2850,8 +2860,9 @@
         <f>[1]summaryCPI!D18</f>
         <v>#REF!</v>
       </c>
-      <c r="P18" s="2">
-        <v>0.52221</v>
+      <c r="P18" s="2" t="e">
+        <f>[1]summaryCPI!C18</f>
+        <v>#REF!</v>
       </c>
       <c r="Q18" s="2">
         <f t="shared" si="12"/>
@@ -2876,7 +2887,7 @@
       <c r="D19" s="5">
         <v>1.181002</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <f t="shared" si="5"/>
         <v>-0.202025675675676</v>
       </c>
@@ -2888,27 +2899,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H19" s="24" t="e">
+      <c r="H19" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I19" s="24" t="e">
+      <c r="I19" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J19" s="36">
+      <c r="J19" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K19" s="36">
+      <c r="K19" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L19" s="36">
+      <c r="L19" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M19" s="50">
+      <c r="M19" s="49">
         <v>0.176099537037037</v>
       </c>
       <c r="N19" s="2" t="e">
@@ -2919,8 +2930,9 @@
         <f>[1]summaryCPI!D19</f>
         <v>#REF!</v>
       </c>
-      <c r="P19" s="2">
-        <v>0.964338</v>
+      <c r="P19" s="2" t="e">
+        <f>[1]summaryCPI!C19</f>
+        <v>#REF!</v>
       </c>
       <c r="Q19" s="2">
         <f t="shared" si="12"/>
@@ -2943,7 +2955,7 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <f t="shared" si="5"/>
         <v>-1</v>
       </c>
@@ -2955,23 +2967,23 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H20" s="24" t="e">
+      <c r="H20" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I20" s="24" t="e">
+      <c r="I20" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J20" s="36">
+      <c r="J20" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K20" s="36">
+      <c r="K20" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L20" s="36">
+      <c r="L20" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2984,8 +2996,9 @@
         <f>[1]summaryCPI!D20</f>
         <v>#REF!</v>
       </c>
-      <c r="P20" s="2">
-        <v>0.423138</v>
+      <c r="P20" s="2" t="e">
+        <f>[1]summaryCPI!C20</f>
+        <v>#REF!</v>
       </c>
       <c r="Q20" s="2">
         <v>0</v>
@@ -3011,7 +3024,7 @@
       <c r="D21" s="5">
         <v>1.250621</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="22">
         <f t="shared" si="5"/>
         <v>-0.193147741935484</v>
       </c>
@@ -3023,27 +3036,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H21" s="24" t="e">
+      <c r="H21" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I21" s="24" t="e">
+      <c r="I21" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J21" s="36">
+      <c r="J21" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K21" s="36">
+      <c r="K21" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L21" s="36">
+      <c r="L21" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M21" s="51">
+      <c r="M21" s="50">
         <v>0.797916666666667</v>
       </c>
       <c r="N21" s="2" t="e">
@@ -3054,8 +3067,9 @@
         <f>[1]summaryCPI!D21</f>
         <v>#REF!</v>
       </c>
-      <c r="P21" s="2">
-        <v>0.740832</v>
+      <c r="P21" s="2" t="e">
+        <f>[1]summaryCPI!C21</f>
+        <v>#REF!</v>
       </c>
       <c r="Q21" s="2">
         <f t="shared" ref="Q21:Q25" si="13">1/D21</f>
@@ -3080,7 +3094,7 @@
       <c r="D22" s="5">
         <v>0.604481</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="22">
         <f t="shared" si="5"/>
         <v>-0.305194252873563</v>
       </c>
@@ -3092,27 +3106,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H22" s="24" t="e">
+      <c r="H22" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I22" s="24" t="e">
+      <c r="I22" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J22" s="36">
+      <c r="J22" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K22" s="36">
+      <c r="K22" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L22" s="36">
+      <c r="L22" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M22" s="52">
+      <c r="M22" s="51">
         <v>1.02019675925926</v>
       </c>
       <c r="N22" s="2" t="e">
@@ -3123,8 +3137,9 @@
         <f>[1]summaryCPI!D22</f>
         <v>#REF!</v>
       </c>
-      <c r="P22" s="2">
-        <v>0.586157</v>
+      <c r="P22" s="2" t="e">
+        <f>[1]summaryCPI!C22</f>
+        <v>#REF!</v>
       </c>
       <c r="Q22" s="2">
         <f t="shared" si="13"/>
@@ -3149,7 +3164,7 @@
       <c r="D23" s="5">
         <v>1.09169</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="22">
         <f t="shared" si="5"/>
         <v>-0.144611165523996</v>
       </c>
@@ -3161,27 +3176,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H23" s="24" t="e">
+      <c r="H23" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I23" s="24" t="e">
+      <c r="I23" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J23" s="36">
+      <c r="J23" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K23" s="36">
+      <c r="K23" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L23" s="36">
+      <c r="L23" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M23" s="52">
+      <c r="M23" s="51">
         <v>6.01892361111111</v>
       </c>
       <c r="N23" s="2" t="e">
@@ -3192,8 +3207,9 @@
         <f>[1]summaryCPI!D23</f>
         <v>#REF!</v>
       </c>
-      <c r="P23" s="2">
-        <v>0.55619</v>
+      <c r="P23" s="2" t="e">
+        <f>[1]summaryCPI!C23</f>
+        <v>#REF!</v>
       </c>
       <c r="Q23" s="2">
         <f t="shared" si="13"/>
@@ -3218,7 +3234,7 @@
       <c r="D24" s="5">
         <v>0.657295</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="22">
         <f t="shared" si="5"/>
         <v>-0.33857106918239</v>
       </c>
@@ -3230,27 +3246,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H24" s="24" t="e">
+      <c r="H24" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I24" s="24" t="e">
+      <c r="I24" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J24" s="36">
+      <c r="J24" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K24" s="36">
+      <c r="K24" s="35">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L24" s="36">
+      <c r="L24" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M24" s="52">
+      <c r="M24" s="51">
         <v>2.46215277777778</v>
       </c>
       <c r="N24" s="2" t="e">
@@ -3261,8 +3277,9 @@
         <f>[1]summaryCPI!D24</f>
         <v>#REF!</v>
       </c>
-      <c r="P24" s="2">
-        <v>1.1409</v>
+      <c r="P24" s="2" t="e">
+        <f>[1]summaryCPI!C24</f>
+        <v>#REF!</v>
       </c>
       <c r="Q24" s="2">
         <f t="shared" si="13"/>
@@ -3289,7 +3306,7 @@
       <c r="D25" s="9">
         <v>1.277799</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="24">
         <f t="shared" si="5"/>
         <v>-0.0170776923076924</v>
       </c>
@@ -3301,27 +3318,27 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="H25" s="24" t="e">
+      <c r="H25" s="23" t="e">
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="I25" s="24" t="e">
+      <c r="I25" s="23" t="e">
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="J25" s="37">
+      <c r="J25" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K25" s="37">
+      <c r="K25" s="36">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L25" s="36">
+      <c r="L25" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M25" s="51">
+      <c r="M25" s="50">
         <v>0.460416666666667</v>
       </c>
       <c r="N25" s="2" t="e">
@@ -3332,8 +3349,9 @@
         <f>[1]summaryCPI!D25</f>
         <v>#REF!</v>
       </c>
-      <c r="P25" s="2">
-        <v>0.59937</v>
+      <c r="P25" s="2" t="e">
+        <f>[1]summaryCPI!C25</f>
+        <v>#REF!</v>
       </c>
       <c r="Q25" s="2">
         <f t="shared" si="13"/>
@@ -3351,20 +3369,19 @@
       <c r="D26" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="26">
-        <f t="array" ref="E26">GEOMEAN(ABS(E2:E25))</f>
-        <v>0.184549597318419</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="38">
-        <f t="array" ref="J26">GEOMEAN(ABS(J2:J25))</f>
-        <v>1</v>
-      </c>
-      <c r="K26" s="26">
-        <f t="array" ref="K26">GEOMEAN(ABS(K2:K25))</f>
+      <c r="E26" s="25">
+        <f t="array" ref="E26">GEOMEAN(ABS(E2:E24))</f>
+        <v>0.20467079709307</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="37">
+        <f t="array" ref="J26">GEOMEAN(ABS(J2:J24))</f>
+        <v>1</v>
+      </c>
+      <c r="K26" s="25">
+        <f t="array" ref="K26">GEOMEAN(ABS(K2:K24))</f>
         <v>1</v>
       </c>
       <c r="L26"/>
@@ -3373,19 +3390,18 @@
       <c r="D27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="27">
         <f t="array" ref="E27">GEOMEAN(ABS(E2:E11))</f>
         <v>0.142217606410036</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="39">
+      <c r="F27" s="20"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="38">
         <f t="array" ref="J27">GEOMEAN(ABS(J2:J11))</f>
         <v>1</v>
       </c>
-      <c r="K27" s="28">
+      <c r="K27" s="27">
         <f t="array" ref="K27">GEOMEAN(ABS(K2:K11))</f>
         <v>1</v>
       </c>
@@ -3395,42 +3411,40 @@
       <c r="D28" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="28">
-        <f t="array" ref="E28">GEOMEAN(ABS(E12:E25))</f>
-        <v>0.22230103537132</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="39">
-        <f t="array" ref="J28">GEOMEAN(ABS(J12:J25))</f>
-        <v>1</v>
-      </c>
-      <c r="K28" s="28">
-        <f t="array" ref="K28">GEOMEAN(ABS(K12:K25))</f>
+      <c r="E28" s="27">
+        <f t="array" ref="E28">GEOMEAN(ABS(E12:E24))</f>
+        <v>0.270815302654283</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="38">
+        <f t="array" ref="J28">GEOMEAN(ABS(J12:J24))</f>
+        <v>1</v>
+      </c>
+      <c r="K28" s="27">
+        <f t="array" ref="K28">GEOMEAN(ABS(K12:K24))</f>
         <v>1</v>
       </c>
       <c r="L28"/>
     </row>
     <row r="29" spans="4:12">
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="28">
-        <f t="array" ref="E29">AVERAGE(ABS(E2:E25))</f>
-        <v>0.292483951415808</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="39">
-        <f t="array" ref="J29">AVERAGE(ABS(J2:J25))</f>
-        <v>1</v>
-      </c>
-      <c r="K29" s="28">
-        <f t="array" ref="K29">AVERAGE(ABS(K2:K25))</f>
+      <c r="E29" s="27">
+        <f t="array" ref="E29">AVERAGE(ABS(E2:E24))</f>
+        <v>0.304458136594422</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="38">
+        <f t="array" ref="J29">AVERAGE(ABS(J2:J24))</f>
+        <v>1</v>
+      </c>
+      <c r="K29" s="27">
+        <f t="array" ref="K29">AVERAGE(ABS(K2:K24))</f>
         <v>1</v>
       </c>
       <c r="L29"/>
@@ -3439,316 +3453,309 @@
       <c r="D30" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="27">
         <f t="array" ref="E30">AVERAGE(ABS(E2:E11))</f>
         <v>0.264676056202914</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="39">
+      <c r="F30" s="20"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="38">
         <f t="array" ref="J30">AVERAGE(ABS(J2:J11))</f>
         <v>1</v>
       </c>
-      <c r="K30" s="28">
+      <c r="K30" s="27">
         <f t="array" ref="K30">AVERAGE(ABS(K2:K11))</f>
         <v>1</v>
       </c>
       <c r="L30"/>
     </row>
     <row r="31" ht="17.55" spans="4:12">
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="29">
-        <f t="array" ref="E31">AVERAGE(ABS(E12:E25))</f>
-        <v>0.312346733710733</v>
-      </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="40">
-        <f t="array" ref="J31">AVERAGE(ABS(J12:J25))</f>
-        <v>1</v>
-      </c>
-      <c r="K31" s="29">
-        <f t="array" ref="K31">AVERAGE(ABS(K12:K25))</f>
+      <c r="E31" s="28">
+        <f t="array" ref="E31">AVERAGE(ABS(E12:E24))</f>
+        <v>0.335059736895582</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="39">
+        <f t="array" ref="J31">AVERAGE(ABS(J12:J24))</f>
+        <v>1</v>
+      </c>
+      <c r="K31" s="28">
+        <f t="array" ref="K31">AVERAGE(ABS(K12:K24))</f>
         <v>1</v>
       </c>
       <c r="L31"/>
     </row>
     <row r="32" spans="6:12">
-      <c r="F32" s="27"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="F32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
       <c r="L32"/>
     </row>
     <row r="33" spans="3:12">
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="30">
-        <f t="array" ref="E33">GEOMEAN(1+ABS(Q2:Q25-R2:R25)/(R2:R25))-1</f>
-        <v>0.315975155537865</v>
-      </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="41" t="e">
-        <f t="array" ref="J33">GEOMEAN(1+ABS(O2:O25-P2:P25)/(P2:P25))-1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K33" s="42" t="e">
-        <f t="array" ref="K33">GEOMEAN(1+ABS(N2:N25-R2:R25)/(R2:R25))-1</f>
+      <c r="E33" s="29">
+        <f t="array" ref="E33">GEOMEAN(1+ABS(Q2:Q24-R2:R24)/(R2:R24))-1</f>
+        <v>0.330782618609708</v>
+      </c>
+      <c r="F33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="40" t="e">
+        <f t="array" ref="J33">GEOMEAN(1+ABS(O2:O24-P2:P24)/(P2:P24))-1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K33" s="41" t="e">
+        <f t="array" ref="K33">GEOMEAN(1+ABS(N2:N24-R2:R24)/(R2:R24))-1</f>
         <v>#REF!</v>
       </c>
       <c r="L33"/>
     </row>
     <row r="34" spans="3:12">
-      <c r="C34" s="16"/>
-      <c r="D34" s="17" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="30">
         <f t="array" ref="E34">GEOMEAN(1+ABS(Q2:Q11-R2:R11)/(R2:R11))-1</f>
         <v>0.231947110984238</v>
       </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="43" t="e">
+      <c r="F34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="42" t="e">
         <f t="array" ref="J34">GEOMEAN(1+ABS(O2:O11-P2:P11)/(P2:P11))-1</f>
         <v>#REF!</v>
       </c>
-      <c r="K34" s="44" t="e">
+      <c r="K34" s="43" t="e">
         <f t="array" ref="K34">GEOMEAN(1+ABS(N2:N11-R2:R11)/(R2:R11))-1</f>
         <v>#REF!</v>
       </c>
       <c r="L34"/>
     </row>
     <row r="35" spans="3:11">
-      <c r="C35" s="18"/>
-      <c r="D35" s="19" t="s">
+      <c r="C35" s="17"/>
+      <c r="D35" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="32">
-        <f t="array" ref="E35">GEOMEAN(1+ABS(Q12:Q25-R12:R25)/(R12:R25))-1</f>
-        <v>0.379481863784545</v>
-      </c>
-      <c r="F35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="45" t="e">
-        <f t="array" ref="J35">GEOMEAN(1+ABS(O12:O25-P12:P25)/(P12:P25))-1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K35" s="46" t="e">
-        <f t="array" ref="K35">GEOMEAN(1+ABS(N12:N25-R12:R25)/(R12:R25))-1</f>
+      <c r="E35" s="31">
+        <f t="array" ref="E35">GEOMEAN(1+ABS(Q12:Q24-R12:R24)/(R12:R24))-1</f>
+        <v>0.41217309369508</v>
+      </c>
+      <c r="F35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="44" t="e">
+        <f t="array" ref="J35">GEOMEAN(1+ABS(O12:O24-P12:P24)/(P12:P24))-1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K35" s="45" t="e">
+        <f t="array" ref="K35">GEOMEAN(1+ABS(N12:N24-R12:R24)/(R12:R24))-1</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="36" spans="3:11">
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="33">
-        <f t="array" ref="E36">AVERAGE(ABS(Q2:Q25-R2:R25))/AVERAGE(R2:R25)</f>
-        <v>0.34726045940567</v>
-      </c>
-      <c r="F36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="14" t="e">
-        <f t="array" ref="J36">AVERAGE(ABS(O2:O25-P2:P25))/AVERAGE(P2:P25)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K36" s="47" t="e">
-        <f t="array" ref="K36">AVERAGE(ABS(N2:N25-R2:R25))/AVERAGE(R2:R25)</f>
+      <c r="E36" s="32">
+        <f t="array" ref="E36">AVERAGE(ABS(Q2:Q24-R2:R24))/AVERAGE(R2:R24)</f>
+        <v>0.358938260512226</v>
+      </c>
+      <c r="F36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="13" t="e">
+        <f t="array" ref="J36">AVERAGE(ABS(O2:O24-P2:P24))/AVERAGE(P2:P24)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K36" s="46" t="e">
+        <f t="array" ref="K36">AVERAGE(ABS(N2:N24-R2:R24))/AVERAGE(R2:R24)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="37" spans="3:11">
-      <c r="C37" s="16"/>
-      <c r="D37" s="21" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="34">
+      <c r="E37" s="33">
         <f t="array" ref="E37">AVERAGE(ABS(Q2:Q11-R2:R11))/AVERAGE(R2:R11)</f>
         <v>0.221166241953315</v>
       </c>
-      <c r="F37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="16" t="e">
+      <c r="F37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="15" t="e">
         <f t="array" ref="J37">AVERAGE(ABS(O2:O11-P2:P11))/AVERAGE(P2:P11)</f>
         <v>#REF!</v>
       </c>
-      <c r="K37" s="48" t="e">
+      <c r="K37" s="47" t="e">
         <f t="array" ref="K37">AVERAGE(ABS(N2:N11-R2:R11))/AVERAGE(R2:R11)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="38" spans="3:11">
-      <c r="C38" s="18"/>
-      <c r="D38" s="22" t="s">
+      <c r="C38" s="17"/>
+      <c r="D38" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="35">
-        <f t="array" ref="E38">AVERAGE(ABS(Q12:Q25-R12:R25))/AVERAGE(R12:R25)</f>
-        <v>0.431499626298951</v>
-      </c>
-      <c r="F38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="18" t="e">
-        <f t="array" ref="J38">AVERAGE(ABS(O12:O25-P12:P25))/AVERAGE(P12:P25)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K38" s="49" t="e">
-        <f t="array" ref="K38">AVERAGE(ABS(N12:N25-R12:R25))/AVERAGE(R12:R25)</f>
+      <c r="E38" s="34">
+        <f t="array" ref="E38">AVERAGE(ABS(Q12:Q24-R12:R24))/AVERAGE(R12:R24)</f>
+        <v>0.456545485863031</v>
+      </c>
+      <c r="F38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="17" t="e">
+        <f t="array" ref="J38">AVERAGE(ABS(O12:O24-P12:P24))/AVERAGE(P12:P24)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K38" s="48" t="e">
+        <f t="array" ref="K38">AVERAGE(ABS(N12:N24-R12:R24))/AVERAGE(R12:R24)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="39" spans="3:11">
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="33">
-        <f t="array" ref="E39">(AVERAGE((Q2:Q25-R2:R25)^2)/AVERAGE((R2:R25)^2))^0.5</f>
-        <v>0.445006570402184</v>
-      </c>
-      <c r="F39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="14" t="e">
-        <f t="array" ref="J39">(AVERAGE((O2:O25-P2:P25)^2)/AVERAGE((P2:P25)^2))^0.5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K39" s="47" t="e">
-        <f t="array" ref="K39">(AVERAGE((N2:N25-R2:R25)^2)/AVERAGE((R2:R25)^2))^0.5</f>
+      <c r="E39" s="32">
+        <f t="array" ref="E39">(AVERAGE((Q2:Q24-R2:R24)^2)/AVERAGE((R2:R24)^2))^0.5</f>
+        <v>0.450634549666886</v>
+      </c>
+      <c r="F39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="13" t="e">
+        <f t="array" ref="J39">(AVERAGE((O2:O24-P2:P24)^2)/AVERAGE((P2:P24)^2))^0.5</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K39" s="46" t="e">
+        <f t="array" ref="K39">(AVERAGE((N2:N24-R2:R24)^2)/AVERAGE((R2:R24)^2))^0.5</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="40" spans="3:11">
-      <c r="C40" s="16"/>
-      <c r="D40" s="21" t="s">
+      <c r="C40" s="15"/>
+      <c r="D40" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E40" s="34">
+      <c r="E40" s="33">
         <f t="array" ref="E40">(AVERAGE((Q2:Q11-R2:R11)^2)/AVERAGE((R2:R11)^2))^0.5</f>
         <v>0.26676163250211</v>
       </c>
-      <c r="F40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="16" t="e">
+      <c r="F40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="15" t="e">
         <f t="array" ref="J40">(AVERAGE((O2:O11-P2:P11)^2)/AVERAGE((P2:P11)^2))^0.5</f>
         <v>#REF!</v>
       </c>
-      <c r="K40" s="48" t="e">
+      <c r="K40" s="47" t="e">
         <f t="array" ref="K40">(AVERAGE((N2:N11-R2:R11)^2)/AVERAGE((R2:R11)^2))^0.5</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="41" spans="3:11">
-      <c r="C41" s="18"/>
-      <c r="D41" s="22" t="s">
+      <c r="C41" s="17"/>
+      <c r="D41" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="35">
-        <f t="array" ref="E41">(AVERAGE((Q12:Q25-R12:R25)^2)/AVERAGE((R12:R25)^2))^0.5</f>
-        <v>0.523477031023408</v>
-      </c>
-      <c r="F41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="18" t="e">
-        <f t="array" ref="J41">(AVERAGE((O12:O25-P12:P25)^2)/AVERAGE((P12:P25)^2))^0.5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K41" s="49" t="e">
-        <f t="array" ref="K41">(AVERAGE((N12:N25-R12:R25)^2)/AVERAGE((R12:R25)^2))^0.5</f>
+      <c r="E41" s="34">
+        <f t="array" ref="E41">(AVERAGE((Q12:Q24-R12:R24)^2)/AVERAGE((R12:R24)^2))^0.5</f>
+        <v>0.53419028085538</v>
+      </c>
+      <c r="F41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="17" t="e">
+        <f t="array" ref="J41">(AVERAGE((O12:O24-P12:P24)^2)/AVERAGE((P12:P24)^2))^0.5</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K41" s="48" t="e">
+        <f t="array" ref="K41">(AVERAGE((N12:N24-R12:R24)^2)/AVERAGE((R12:R24)^2))^0.5</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="42" spans="3:11">
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="33">
-        <f t="array" ref="E42">AVERAGE(ABS(Q2:Q25-R2:R25)/(R2:R25))</f>
-        <v>0.348394362956864</v>
-      </c>
-      <c r="F42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="14" t="e">
-        <f t="array" ref="J42">AVERAGE(ABS(O2:O25-P2:P25)/(P2:P25))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K42" s="47" t="e">
-        <f t="array" ref="K42">AVERAGE(ABS(N2:N25-R2:R25)/(R2:R25))</f>
+      <c r="E42" s="32">
+        <f t="array" ref="E42">AVERAGE(ABS(Q2:Q24-R2:R24)/(R2:R24))</f>
+        <v>0.362786534951252</v>
+      </c>
+      <c r="F42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="13" t="e">
+        <f t="array" ref="J42">AVERAGE(ABS(O2:O24-P2:P24)/(P2:P24))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K42" s="46" t="e">
+        <f t="array" ref="K42">AVERAGE(ABS(N2:N24-R2:R24)/(R2:R24))</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="43" spans="3:11">
-      <c r="C43" s="16"/>
-      <c r="D43" s="21" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E43" s="33">
         <f t="array" ref="E43">AVERAGE(ABS(Q2:Q11-R2:R11)/(R2:R11))</f>
         <v>0.254886723228489</v>
       </c>
-      <c r="F43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="16" t="e">
+      <c r="F43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="15" t="e">
         <f t="array" ref="J43">AVERAGE(ABS(O2:O11-P2:P11)/(P2:P11))</f>
         <v>#REF!</v>
       </c>
-      <c r="K43" s="48" t="e">
+      <c r="K43" s="47" t="e">
         <f t="array" ref="K43">AVERAGE(ABS(N2:N11-R2:R11)/(R2:R11))</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="44" spans="3:11">
-      <c r="C44" s="18"/>
-      <c r="D44" s="22" t="s">
+      <c r="C44" s="17"/>
+      <c r="D44" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="35">
-        <f t="array" ref="E44">AVERAGE(ABS(Q12:Q25-R12:R25)/(R12:R25))</f>
-        <v>0.415185534191417</v>
-      </c>
-      <c r="F44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="18" t="e">
-        <f t="array" ref="J44">AVERAGE(ABS(O12:O25-P12:P25)/(P12:P25))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K44" s="49" t="e">
-        <f t="array" ref="K44">AVERAGE(ABS(N12:N25-R12:R25)/(R12:R25))</f>
+      <c r="E44" s="34">
+        <f t="array" ref="E44">AVERAGE(ABS(Q12:Q24-R12:R24)/(R12:R24))</f>
+        <v>0.445786390122607</v>
+      </c>
+      <c r="F44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="17" t="e">
+        <f t="array" ref="J44">AVERAGE(ABS(O12:O24-P12:P24)/(P12:P24))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K44" s="48" t="e">
+        <f t="array" ref="K44">AVERAGE(ABS(N12:N24-R12:R24)/(R12:R24))</f>
         <v>#REF!</v>
       </c>
     </row>

</xml_diff>